<commit_message>
Copy uploaded file as a backup
</commit_message>
<xml_diff>
--- a/src/main/resources/minister-template.xlsx
+++ b/src/main/resources/minister-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -85,6 +85,12 @@
     <t xml:space="preserve">PartyImageUrl</t>
   </si>
   <si>
+    <t xml:space="preserve">Constituency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mr</t>
   </si>
   <si>
@@ -122,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">http://localhost:1337/assets/images/IndianNationalCongress.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pimpri Chinchwad</t>
   </si>
 </sst>
 </file>
@@ -131,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -233,6 +248,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -382,8 +402,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,10 +504,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -509,7 +533,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="49.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="52.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,49 +601,61 @@
       <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>101</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,43 +663,49 @@
         <v>102</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>